<commit_message>
Added "reel" as top container drop down
</commit_message>
<xml_diff>
--- a/aspace_excel_importer/aspace_import_excel_template_cul.xlsx
+++ b/aspace_excel_importer/aspace_import_excel_template_cul.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="268">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -805,18 +805,6 @@
   </si>
   <si>
     <t>Extent type (not required)</t>
-  </si>
-  <si>
-    <t>Purchased</t>
-  </si>
-  <si>
-    <t>In alphabetical order</t>
-  </si>
-  <si>
-    <t>In English</t>
-  </si>
-  <si>
-    <t>Photocopied on thermal paper</t>
   </si>
   <si>
     <t>This is the template for importing using aspace-import-excel, lightly modifed for Columbia University Libraries.  You may replace this line with something of your choosing after you've copied the file for your use.</t>
@@ -1721,7 +1709,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,7 +1778,7 @@
   <sheetData>
     <row r="1" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:79" s="1" customFormat="1" ht="51.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2104,7 +2092,7 @@
         <v>37</v>
       </c>
       <c r="Y3" s="52" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="Z3" s="52" t="s">
         <v>223</v>
@@ -2113,10 +2101,10 @@
         <v>95</v>
       </c>
       <c r="AB3" s="65" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AC3" s="55" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="AD3" s="55" t="s">
         <v>93</v>
@@ -2749,7 +2737,7 @@
     </row>
     <row r="6" spans="1:79" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>248</v>
@@ -2775,7 +2763,7 @@
     </row>
     <row r="7" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>249</v>
@@ -2813,7 +2801,7 @@
     </row>
     <row r="8" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>250</v>
@@ -2828,10 +2816,10 @@
         <v>1</v>
       </c>
       <c r="N8" s="53" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="Q8" s="53" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Y8" s="1" t="s">
         <v>237</v>
@@ -2851,7 +2839,7 @@
     </row>
     <row r="9" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>251</v>
@@ -2889,7 +2877,7 @@
     </row>
     <row r="10" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>252</v>
@@ -2927,7 +2915,7 @@
     </row>
     <row r="11" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>253</v>
@@ -2968,7 +2956,7 @@
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>230</v>
@@ -2990,23 +2978,11 @@
       </c>
       <c r="Q12" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="BL12" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="BM12" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="BR12" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="BW12" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>254</v>
@@ -3044,7 +3020,7 @@
     </row>
     <row r="14" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>255</v>
@@ -3082,7 +3058,7 @@
     </row>
     <row r="15" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>256</v>
@@ -3119,7 +3095,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H1048576">
       <formula1>"Class,Collection,File,Fonds,Item,Other Level,Record Group,Series,Sub-Fonds,Sub-Group,Sub-Series"</formula1>
     </dataValidation>
@@ -3136,8 +3112,11 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y6:Y1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y728:Y1048576">
       <formula1>"box, accession, add box, album, audio, binder, book, drawer, flat box, folder, item, ledger, mapcase, microfilm, oversize box, tube box, volume"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y6:Y727">
+      <formula1>"box, accession, add box, album, audio, binder, book, drawer, flat box, folder, item, ledger, mapcase, microfilm, oversize box, reel, tube box, volume"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
updated controlled container and extent lists
</commit_message>
<xml_diff>
--- a/aspace_excel_importer/aspace_import_excel_template_cul.xlsx
+++ b/aspace_excel_importer/aspace_import_excel_template_cul.xlsx
@@ -10,12 +10,17 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Documentation" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="audio_cylinders">Documentation!$B$2:$B$25</definedName>
+    <definedName name="column_U_control_list">Documentation!$B$2:$B$21</definedName>
+    <definedName name="column_Y_control_list">Documentation!$C$2:$C$19</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="311">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -102,9 +107,6 @@
   </si>
   <si>
     <t>Dates Type</t>
-  </si>
-  <si>
-    <t>Extent type: cubic feet, cds, etc.</t>
   </si>
   <si>
     <t>Top Container type</t>
@@ -802,9 +804,6 @@
   </si>
   <si>
     <t>Extent number (not required)</t>
-  </si>
-  <si>
-    <t>Extent type (not required)</t>
   </si>
   <si>
     <t>This is the template for importing using aspace-import-excel, lightly modifed for Columbia University Libraries.  You may replace this line with something of your choosing after you've copied the file for your use.</t>
@@ -839,18 +838,160 @@
   <si>
     <t>Child container type; folder, item, etc.</t>
   </si>
+  <si>
+    <t>Extent type (not required). Controlled by AS extent_extent_type vocabulary</t>
+  </si>
+  <si>
+    <t>Extent type: linear feet, audiocassettes, etc.</t>
+  </si>
+  <si>
+    <t>items</t>
+  </si>
+  <si>
+    <t>boxes</t>
+  </si>
+  <si>
+    <t>linear feet</t>
+  </si>
+  <si>
+    <t>audio cylinders</t>
+  </si>
+  <si>
+    <t>audiocassettes</t>
+  </si>
+  <si>
+    <t>compact disks</t>
+  </si>
+  <si>
+    <t>digital audio files (Sound recordings)</t>
+  </si>
+  <si>
+    <t>film reels</t>
+  </si>
+  <si>
+    <t>filmstrips</t>
+  </si>
+  <si>
+    <t>open reel audiotapes</t>
+  </si>
+  <si>
+    <t>pages</t>
+  </si>
+  <si>
+    <t>phonograph records</t>
+  </si>
+  <si>
+    <t>reels</t>
+  </si>
+  <si>
+    <t>sheets</t>
+  </si>
+  <si>
+    <t>videocassettes (U-matic)</t>
+  </si>
+  <si>
+    <t>videocassettes (VHS)</t>
+  </si>
+  <si>
+    <t>videotape</t>
+  </si>
+  <si>
+    <t>volumes</t>
+  </si>
+  <si>
+    <t>accession</t>
+  </si>
+  <si>
+    <t>add box</t>
+  </si>
+  <si>
+    <t>album</t>
+  </si>
+  <si>
+    <t>audio</t>
+  </si>
+  <si>
+    <t>binder</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>drawer</t>
+  </si>
+  <si>
+    <t>flatbox</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>ledger</t>
+  </si>
+  <si>
+    <t>mapcase</t>
+  </si>
+  <si>
+    <t>microfilm</t>
+  </si>
+  <si>
+    <t>oversize box</t>
+  </si>
+  <si>
+    <t>reel</t>
+  </si>
+  <si>
+    <t>tube box</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>column_U_control_list</t>
+  </si>
+  <si>
+    <t>column_Y_control_list</t>
+  </si>
+  <si>
+    <t>Beta (Betamax)</t>
+  </si>
+  <si>
+    <t>digital audio tapes</t>
+  </si>
+  <si>
+    <t>DVDs</t>
+  </si>
+  <si>
+    <t>microcassettes</t>
+  </si>
+  <si>
+    <t>Mini-DVs</t>
+  </si>
+  <si>
+    <t>folders</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -1129,150 +1270,151 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1280,59 +1422,63 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1410,9 +1556,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1709,7 +1852,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,7 +1921,7 @@
   <sheetData>
     <row r="1" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:79" s="1" customFormat="1" ht="51.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1786,109 +1929,109 @@
         <v>0</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K2" s="45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N2" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O2" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q2" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R2" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U2" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="V2" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Y2" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA2" s="54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB2" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AC2" s="54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AD2" s="54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AE2" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AF2" s="54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AG2" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AH2" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AI2" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AJ2" s="51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AK2" s="20" t="s">
         <v>1</v>
@@ -1942,118 +2085,118 @@
         <v>1</v>
       </c>
       <c r="BB2" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="BC2" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="BD2" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="BE2" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="BF2" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="BG2" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="BH2" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="BI2" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="BJ2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BK2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BL2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BM2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BN2" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BO2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BP2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BQ2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BR2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BS2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BT2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BU2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BV2" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BW2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BX2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BY2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BZ2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="CA2" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:79" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>229</v>
-      </c>
       <c r="F3" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K3" s="46" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M3" s="62" t="s">
         <v>19</v>
@@ -2065,196 +2208,196 @@
         <v>17</v>
       </c>
       <c r="P3" s="62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="R3" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="S3" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="T3" s="63" t="s">
+        <v>258</v>
+      </c>
+      <c r="U3" s="63" t="s">
+        <v>266</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="W3" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="S3" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="T3" s="63" t="s">
-        <v>259</v>
-      </c>
-      <c r="U3" s="63" t="s">
+      <c r="X3" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y3" s="52" t="s">
+        <v>264</v>
+      </c>
+      <c r="Z3" s="52" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA3" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB3" s="65" t="s">
         <v>260</v>
       </c>
-      <c r="V3" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="W3" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="X3" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y3" s="52" t="s">
-        <v>266</v>
-      </c>
-      <c r="Z3" s="52" t="s">
-        <v>223</v>
-      </c>
-      <c r="AA3" s="57" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB3" s="65" t="s">
-        <v>262</v>
-      </c>
       <c r="AC3" s="55" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="AD3" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE3" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF3" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="AE3" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF3" s="55" t="s">
-        <v>94</v>
-      </c>
       <c r="AG3" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH3" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AI3" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AJ3" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="AK3" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="AL3" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM3" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="AN3" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO3" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="AP3" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="AQ3" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="AR3" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="AS3" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="AK3" s="28" t="s">
+      <c r="AT3" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="AL3" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="AM3" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="AN3" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="AO3" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="AP3" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="AQ3" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="AR3" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="AS3" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="AT3" s="28" t="s">
+      <c r="AU3" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="AV3" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="AW3" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="AU3" s="28" t="s">
+      <c r="AX3" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="AY3" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="AV3" s="28" t="s">
+      <c r="AZ3" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="BA3" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="AW3" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="AX3" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="AY3" s="28" t="s">
-        <v>194</v>
-      </c>
-      <c r="AZ3" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="BA3" s="28" t="s">
-        <v>195</v>
-      </c>
       <c r="BB3" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BC3" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="BD3" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="BD3" s="28" t="s">
-        <v>124</v>
-      </c>
       <c r="BE3" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BF3" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BG3" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="BH3" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="BH3" s="28" t="s">
-        <v>124</v>
-      </c>
       <c r="BI3" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BJ3" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="BK3" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="BK3" s="27" t="s">
+      <c r="BL3" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="BL3" s="27" t="s">
+      <c r="BM3" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="BM3" s="27" t="s">
+      <c r="BN3" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="BN3" s="27" t="s">
+      <c r="BO3" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="BO3" s="27" t="s">
+      <c r="BP3" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="BP3" s="27" t="s">
+      <c r="BQ3" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="BQ3" s="27" t="s">
-        <v>148</v>
-      </c>
       <c r="BR3" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="BS3" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="BS3" s="27" t="s">
-        <v>151</v>
-      </c>
       <c r="BT3" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="BU3" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="BU3" s="27" t="s">
+      <c r="BV3" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="BV3" s="27" t="s">
+      <c r="BW3" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="BW3" s="27" t="s">
+      <c r="BX3" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="BX3" s="27" t="s">
-        <v>157</v>
-      </c>
       <c r="BY3" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BZ3" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="CA3" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:79" s="44" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2265,37 +2408,37 @@
         <v>5</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" s="40" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4" s="40" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J4" s="40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K4" s="47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L4" s="40" t="s">
         <v>7</v>
       </c>
       <c r="M4" s="40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N4" s="42" t="s">
         <v>24</v>
@@ -2310,10 +2453,10 @@
         <v>23</v>
       </c>
       <c r="R4" s="40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S4" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T4" s="40" t="s">
         <v>22</v>
@@ -2322,16 +2465,16 @@
         <v>13</v>
       </c>
       <c r="V4" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="W4" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X4" s="43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y4" s="40" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Z4" s="40" t="s">
         <v>8</v>
@@ -2340,7 +2483,7 @@
         <v>9</v>
       </c>
       <c r="AB4" s="40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AC4" s="42" t="s">
         <v>10</v>
@@ -2349,192 +2492,192 @@
         <v>11</v>
       </c>
       <c r="AE4" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF4" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="AF4" s="42" t="s">
-        <v>35</v>
-      </c>
       <c r="AG4" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH4" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI4" s="40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AJ4" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="AK4" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="AL4" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="AM4" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="AN4" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="AO4" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="AP4" s="40" t="s">
+        <v>204</v>
+      </c>
+      <c r="AQ4" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="AR4" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="AS4" s="40" t="s">
         <v>217</v>
       </c>
-      <c r="AK4" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="AL4" s="40" t="s">
-        <v>201</v>
-      </c>
-      <c r="AM4" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="AN4" s="40" t="s">
-        <v>203</v>
-      </c>
-      <c r="AO4" s="40" t="s">
-        <v>204</v>
-      </c>
-      <c r="AP4" s="40" t="s">
-        <v>205</v>
-      </c>
-      <c r="AQ4" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="AR4" s="40" t="s">
+      <c r="AT4" s="40" t="s">
+        <v>218</v>
+      </c>
+      <c r="AU4" s="40" t="s">
+        <v>219</v>
+      </c>
+      <c r="AV4" s="40" t="s">
         <v>207</v>
       </c>
-      <c r="AS4" s="40" t="s">
-        <v>218</v>
-      </c>
-      <c r="AT4" s="40" t="s">
-        <v>219</v>
-      </c>
-      <c r="AU4" s="40" t="s">
-        <v>220</v>
-      </c>
-      <c r="AV4" s="40" t="s">
+      <c r="AW4" s="40" t="s">
         <v>208</v>
       </c>
-      <c r="AW4" s="40" t="s">
+      <c r="AX4" s="40" t="s">
         <v>209</v>
       </c>
-      <c r="AX4" s="40" t="s">
+      <c r="AY4" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="AY4" s="40" t="s">
+      <c r="AZ4" s="40" t="s">
+        <v>212</v>
+      </c>
+      <c r="BA4" s="40" t="s">
         <v>211</v>
       </c>
-      <c r="AZ4" s="40" t="s">
-        <v>213</v>
-      </c>
-      <c r="BA4" s="40" t="s">
-        <v>212</v>
-      </c>
       <c r="BB4" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="BC4" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="BD4" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="BE4" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="BF4" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="BC4" s="40" t="s">
-        <v>125</v>
-      </c>
-      <c r="BD4" s="40" t="s">
+      <c r="BG4" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="BE4" s="40" t="s">
+      <c r="BH4" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="BI4" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="BF4" s="40" t="s">
-        <v>171</v>
-      </c>
-      <c r="BG4" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="BH4" s="40" t="s">
-        <v>128</v>
-      </c>
-      <c r="BI4" s="40" t="s">
-        <v>173</v>
-      </c>
       <c r="BJ4" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="BK4" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL4" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="BM4" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="BN4" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="BO4" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="BP4" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="BQ4" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="BR4" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="BS4" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="BT4" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="BU4" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="BV4" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="BW4" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="BK4" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="BL4" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="BM4" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="BN4" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="BO4" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="BP4" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="BQ4" s="43" t="s">
+      <c r="BX4" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="BY4" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="BZ4" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="BR4" s="43" t="s">
+      <c r="CA4" s="43" t="s">
         <v>61</v>
-      </c>
-      <c r="BS4" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="BT4" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="BU4" s="40" t="s">
-        <v>118</v>
-      </c>
-      <c r="BV4" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="BW4" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="BX4" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="BY4" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="BZ4" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="CA4" s="43" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:79" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="61" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="K5" s="49" t="s">
         <v>165</v>
-      </c>
-      <c r="K5" s="49" t="s">
-        <v>166</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N5" s="56" t="s">
         <v>26</v>
@@ -2549,553 +2692,553 @@
         <v>18</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T5" s="64" t="s">
         <v>21</v>
       </c>
       <c r="U5" s="64" t="s">
-        <v>29</v>
+        <v>267</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="X5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="Y5" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AA5" s="56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AB5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC5" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="AC5" s="56" t="s">
-        <v>33</v>
-      </c>
       <c r="AD5" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF5" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="AE5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF5" s="56" t="s">
-        <v>92</v>
-      </c>
       <c r="AG5" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AH5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AI5" s="4" t="s">
+      <c r="AJ5" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AL5" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="AM5" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AN5" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AO5" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AP5" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="AQ5" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AR5" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="AS5" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="AT5" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="AU5" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AV5" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AW5" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AX5" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="AY5" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="AZ5" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="BA5" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="BB5" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="BC5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="BD5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="BE5" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="BF5" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="BG5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="BH5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="BI5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="BJ5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="BK5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="BL5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="BM5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="BN5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AJ5" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="AK5" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="AL5" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AM5" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="AN5" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AO5" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="AP5" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="AQ5" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="AR5" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="AS5" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="AT5" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="AU5" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="AV5" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="AW5" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="AX5" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="AY5" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="AZ5" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="BA5" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="BB5" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="BC5" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="BD5" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="BE5" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="BF5" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="BG5" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="BH5" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="BI5" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="BJ5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="BK5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="BL5" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="BM5" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="BN5" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="BO5" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BP5" s="39" t="s">
         <v>3</v>
       </c>
       <c r="BQ5" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BR5" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BS5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="BT5" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BU5" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="BV5" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="BW5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BX5" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BY5" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="BZ5" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="CA5" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:79" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J6" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N6" s="53" t="s">
+        <v>232</v>
+      </c>
+      <c r="O6" s="53" t="s">
         <v>233</v>
       </c>
-      <c r="O6" s="53" t="s">
+      <c r="Q6" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G7" s="33">
         <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N7" s="53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q7" s="53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Y7" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="AA7" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="Z7" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="AA7" s="53" t="s">
+      <c r="AC7" s="53" t="s">
         <v>238</v>
       </c>
-      <c r="AC7" s="53" t="s">
+      <c r="AD7" s="53" t="s">
         <v>239</v>
-      </c>
-      <c r="AD7" s="53" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G8" s="33">
         <v>2</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J8" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N8" s="53" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="Q8" s="53" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="Y8" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="AA8" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="Z8" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="AA8" s="53" t="s">
+      <c r="AC8" s="53" t="s">
         <v>238</v>
       </c>
-      <c r="AC8" s="53" t="s">
-        <v>239</v>
-      </c>
       <c r="AD8" s="53" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G9" s="33">
         <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N9" s="53" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q9" s="53" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Y9" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="AA9" s="53" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC9" s="53" t="s">
+        <v>238</v>
+      </c>
+      <c r="AD9" s="53" t="s">
         <v>237</v>
-      </c>
-      <c r="Z9" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="AA9" s="53" t="s">
-        <v>242</v>
-      </c>
-      <c r="AC9" s="53" t="s">
-        <v>239</v>
-      </c>
-      <c r="AD9" s="53" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G10" s="33">
         <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J10" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N10" s="53" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Q10" s="53" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA10" s="53" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AC10" s="53" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AD10" s="53" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G11" s="33">
         <v>2</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J11" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N11" s="53" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O11" s="53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q11" s="53" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA11" s="53" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC11" s="53" t="s">
+        <v>238</v>
+      </c>
+      <c r="AD11" s="53" t="s">
         <v>242</v>
-      </c>
-      <c r="AC11" s="53" t="s">
-        <v>239</v>
-      </c>
-      <c r="AD11" s="53" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J12" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N12" s="53" t="s">
+        <v>256</v>
+      </c>
+      <c r="O12" s="53" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="O12" s="53" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G13" s="33">
         <v>2</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J13" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N13" s="53" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q13" s="53" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Y13" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="AA13" s="53" t="s">
+        <v>242</v>
+      </c>
+      <c r="AC13" s="53" t="s">
+        <v>238</v>
+      </c>
+      <c r="AD13" s="53" t="s">
         <v>237</v>
-      </c>
-      <c r="Z13" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="AA13" s="53" t="s">
-        <v>243</v>
-      </c>
-      <c r="AC13" s="53" t="s">
-        <v>239</v>
-      </c>
-      <c r="AD13" s="53" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G14" s="33">
         <v>2</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J14" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N14" s="53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q14" s="53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA14" s="53" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AC14" s="53" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AD14" s="53" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G15" s="33">
         <v>2</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J15" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N15" s="53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q15" s="53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA15" s="53" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AC15" s="53" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AD15" s="53" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="7">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H1048576">
       <formula1>"Class,Collection,File,Fonds,Item,Other Level,Record Group,Series,Sub-Fonds,Sub-Group,Sub-Series"</formula1>
     </dataValidation>
@@ -3112,70 +3255,247 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y728:Y1048576">
-      <formula1>"box, accession, add box, album, audio, binder, book, drawer, flat box, folder, item, ledger, mapcase, microfilm, oversize box, tube box, volume"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y6:Y727">
-      <formula1>"box, accession, add box, album, audio, binder, book, drawer, flat box, folder, item, ledger, mapcase, microfilm, oversize box, reel, tube box, volume"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y6:Y1048576">
+      <formula1>column_Y_control_list</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Documentation!$B$2:$B$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>U6:U1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="128.28515625" customWidth="1"/>
-    <col min="2" max="1025" width="8.5703125"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="66" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="68" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="66" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" s="66" t="s">
+        <v>305</v>
+      </c>
+      <c r="C4" s="68" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" s="66" t="s">
+        <v>269</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" s="66" t="s">
+        <v>273</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="50" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="B7" s="66" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="68" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" s="66" t="s">
+        <v>306</v>
+      </c>
+      <c r="C8" s="68" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="B9" s="66" t="s">
+        <v>307</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="66" t="s">
+        <v>275</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="66" t="s">
+        <v>276</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="67" t="s">
+        <v>310</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="66" t="s">
+        <v>268</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="66" t="s">
+        <v>270</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="66" t="s">
+        <v>308</v>
+      </c>
+      <c r="C15" s="68" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="66" t="s">
+        <v>309</v>
+      </c>
+      <c r="C16" s="68" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="66" t="s">
+        <v>277</v>
+      </c>
+      <c r="C17" s="68" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="66" t="s">
+        <v>278</v>
+      </c>
+      <c r="C18" s="68" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="66" t="s">
+        <v>279</v>
+      </c>
+      <c r="C19" s="68" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="66" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="66" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>